<commit_message>
Lập danh sách + Chọn quà
</commit_message>
<xml_diff>
--- a/src/CreateList/Write.xlsx
+++ b/src/CreateList/Write.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -47,42 +47,48 @@
     <t>8</t>
   </si>
   <si>
+    <t>Học sinh giỏi</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Vũ Tiến Hùng</t>
+  </si>
+  <si>
+    <t>2009-10-18</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>Thành tích đặc biệt</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Vũ Tiến Hùng</t>
-  </si>
-  <si>
-    <t>2009-10-18</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>Vũ Tiến Thành</t>
+  </si>
+  <si>
+    <t>2015-10-02</t>
+  </si>
+  <si>
+    <t>Trường Tiểu học Bắc Sơn</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Lan Anh</t>
+  </si>
+  <si>
+    <t>2008-06-19</t>
+  </si>
+  <si>
+    <t>Trường THCS Sầm Sơn</t>
   </si>
   <si>
     <t>Học sinh tiên tiến</t>
   </si>
   <si>
-    <t>Vũ Tiến Thành</t>
-  </si>
-  <si>
-    <t>2015-10-02</t>
-  </si>
-  <si>
-    <t>Trường Tiểu học Bắc Sơn</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Lan Anh</t>
-  </si>
-  <si>
-    <t>2008-06-19</t>
-  </si>
-  <si>
-    <t>Trường THCS Sầm Sơn</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -96,9 +102,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>Không</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -246,22 +249,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -269,22 +272,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>